<commit_message>
added drafted , subject line columns, clean email body wihtout gemini extrea text
</commit_message>
<xml_diff>
--- a/apollo_data.xlsx
+++ b/apollo_data.xlsx
@@ -8933,7 +8933,7 @@
     <col customWidth="1" min="2" max="2" width="47.63"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -8949,7 +8949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -8981,7 +8981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -8997,7 +8997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -9037,7 +9037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>

</xml_diff>